<commit_message>
Wrote a script to collect output
</commit_message>
<xml_diff>
--- a/matcher/out/Workbook1.xlsx
+++ b/matcher/out/Workbook1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38280" windowHeight="20820" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="237">
   <si>
     <t>total_score</t>
   </si>
@@ -780,6 +780,12 @@
   </si>
   <si>
     <t>1lj8374h</t>
+  </si>
+  <si>
+    <t>mutant</t>
+  </si>
+  <si>
+    <t>scaffold</t>
   </si>
 </sst>
 </file>
@@ -1216,8 +1222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AM18" sqref="AM18"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="AR2" sqref="AR2:AR164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1393,7 +1399,10 @@
         <v>204</v>
       </c>
       <c r="AQ1" s="2" t="s">
-        <v>204</v>
+        <v>235</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:44">
@@ -1526,8 +1535,9 @@
       <c r="AQ2" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="AR2">
-        <v>4</v>
+      <c r="AR2" t="str">
+        <f>MID(AP2,1,4)</f>
+        <v>1kol</v>
       </c>
     </row>
     <row r="3" spans="1:44">
@@ -1660,8 +1670,9 @@
       <c r="AQ3" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="AR3">
-        <v>1</v>
+      <c r="AR3" t="str">
+        <f t="shared" ref="AR3:AR66" si="0">MID(AP3,1,4)</f>
+        <v>1kol</v>
       </c>
     </row>
     <row r="4" spans="1:44">
@@ -1794,8 +1805,9 @@
       <c r="AQ4" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="AR4">
-        <v>2</v>
+      <c r="AR4" t="str">
+        <f t="shared" si="0"/>
+        <v>1kol</v>
       </c>
     </row>
     <row r="5" spans="1:44">
@@ -1928,8 +1940,9 @@
       <c r="AQ5" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="AR5">
-        <v>6</v>
+      <c r="AR5" t="str">
+        <f t="shared" si="0"/>
+        <v>1kol</v>
       </c>
     </row>
     <row r="6" spans="1:44">
@@ -2062,8 +2075,9 @@
       <c r="AQ6" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="AR6">
-        <v>3</v>
+      <c r="AR6" t="str">
+        <f t="shared" si="0"/>
+        <v>1kol</v>
       </c>
     </row>
     <row r="7" spans="1:44">
@@ -2196,8 +2210,9 @@
       <c r="AQ7" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="AR7">
-        <v>5</v>
+      <c r="AR7" t="str">
+        <f t="shared" si="0"/>
+        <v>1kol</v>
       </c>
     </row>
     <row r="8" spans="1:44">
@@ -2330,8 +2345,9 @@
       <c r="AQ8" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="AR8">
-        <v>5</v>
+      <c r="AR8" t="str">
+        <f t="shared" si="0"/>
+        <v>1lj8</v>
       </c>
     </row>
     <row r="9" spans="1:44">
@@ -2464,8 +2480,9 @@
       <c r="AQ9" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="AR9">
-        <v>1</v>
+      <c r="AR9" t="str">
+        <f t="shared" si="0"/>
+        <v>1lj8</v>
       </c>
     </row>
     <row r="10" spans="1:44">
@@ -2598,8 +2615,9 @@
       <c r="AQ10" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="AR10">
-        <v>2</v>
+      <c r="AR10" t="str">
+        <f t="shared" si="0"/>
+        <v>1lj8</v>
       </c>
     </row>
     <row r="11" spans="1:44">
@@ -2732,8 +2750,9 @@
       <c r="AQ11" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="AR11">
-        <v>4</v>
+      <c r="AR11" t="str">
+        <f t="shared" si="0"/>
+        <v>1lj8</v>
       </c>
     </row>
     <row r="12" spans="1:44">
@@ -2866,8 +2885,9 @@
       <c r="AQ12" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="AR12">
-        <v>9</v>
+      <c r="AR12" t="str">
+        <f t="shared" si="0"/>
+        <v>1lj8</v>
       </c>
     </row>
     <row r="13" spans="1:44">
@@ -3000,8 +3020,9 @@
       <c r="AQ13" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="AR13">
-        <v>7</v>
+      <c r="AR13" t="str">
+        <f t="shared" si="0"/>
+        <v>1lj8</v>
       </c>
     </row>
     <row r="14" spans="1:44">
@@ -3134,8 +3155,9 @@
       <c r="AQ14" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="AR14">
-        <v>5</v>
+      <c r="AR14" t="str">
+        <f t="shared" si="0"/>
+        <v>1lj8</v>
       </c>
     </row>
     <row r="15" spans="1:44">
@@ -3268,8 +3290,9 @@
       <c r="AQ15" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="AR15">
-        <v>1</v>
+      <c r="AR15" t="str">
+        <f t="shared" si="0"/>
+        <v>1lj8</v>
       </c>
     </row>
     <row r="16" spans="1:44">
@@ -3402,8 +3425,9 @@
       <c r="AQ16" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="AR16">
-        <v>1</v>
+      <c r="AR16" t="str">
+        <f t="shared" si="0"/>
+        <v>1lj8</v>
       </c>
     </row>
     <row r="17" spans="1:44">
@@ -3536,8 +3560,9 @@
       <c r="AQ17" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="AR17">
-        <v>4</v>
+      <c r="AR17" t="str">
+        <f t="shared" si="0"/>
+        <v>1nnu</v>
       </c>
     </row>
     <row r="18" spans="1:44">
@@ -3670,8 +3695,9 @@
       <c r="AQ18" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="AR18">
-        <v>3</v>
+      <c r="AR18" t="str">
+        <f t="shared" si="0"/>
+        <v>1nnu</v>
       </c>
     </row>
     <row r="19" spans="1:44">
@@ -3804,8 +3830,9 @@
       <c r="AQ19" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="AR19">
-        <v>5</v>
+      <c r="AR19" t="str">
+        <f t="shared" si="0"/>
+        <v>1nnu</v>
       </c>
     </row>
     <row r="20" spans="1:44">
@@ -3938,8 +3965,9 @@
       <c r="AQ20" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="AR20">
-        <v>6</v>
+      <c r="AR20" t="str">
+        <f t="shared" si="0"/>
+        <v>1nnu</v>
       </c>
     </row>
     <row r="21" spans="1:44">
@@ -4072,8 +4100,9 @@
       <c r="AQ21" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="AR21">
-        <v>1</v>
+      <c r="AR21" t="str">
+        <f t="shared" si="0"/>
+        <v>1nnu</v>
       </c>
     </row>
     <row r="22" spans="1:44">
@@ -4206,8 +4235,9 @@
       <c r="AQ22" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="AR22">
-        <v>8</v>
+      <c r="AR22" t="str">
+        <f t="shared" si="0"/>
+        <v>1nnu</v>
       </c>
     </row>
     <row r="23" spans="1:44">
@@ -4340,8 +4370,9 @@
       <c r="AQ23" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="AR23">
-        <v>2</v>
+      <c r="AR23" t="str">
+        <f t="shared" si="0"/>
+        <v>1nnu</v>
       </c>
     </row>
     <row r="24" spans="1:44">
@@ -4474,8 +4505,9 @@
       <c r="AQ24" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="AR24">
-        <v>9</v>
+      <c r="AR24" t="str">
+        <f t="shared" si="0"/>
+        <v>1nnu</v>
       </c>
     </row>
     <row r="25" spans="1:44">
@@ -4608,8 +4640,9 @@
       <c r="AQ25" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="AR25">
-        <v>7</v>
+      <c r="AR25" t="str">
+        <f t="shared" si="0"/>
+        <v>1nnu</v>
       </c>
     </row>
     <row r="26" spans="1:44">
@@ -4742,8 +4775,9 @@
       <c r="AQ26" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="AR26">
-        <v>2</v>
+      <c r="AR26" t="str">
+        <f t="shared" si="0"/>
+        <v>1nnu</v>
       </c>
     </row>
     <row r="27" spans="1:44">
@@ -4876,8 +4910,9 @@
       <c r="AQ27" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="AR27">
-        <v>5</v>
+      <c r="AR27" t="str">
+        <f t="shared" si="0"/>
+        <v>1nnu</v>
       </c>
     </row>
     <row r="28" spans="1:44">
@@ -5010,8 +5045,9 @@
       <c r="AQ28" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="AR28">
-        <v>3</v>
+      <c r="AR28" t="str">
+        <f t="shared" si="0"/>
+        <v>1nnu</v>
       </c>
     </row>
     <row r="29" spans="1:44">
@@ -5144,8 +5180,9 @@
       <c r="AQ29" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="AR29">
-        <v>4</v>
+      <c r="AR29" t="str">
+        <f t="shared" si="0"/>
+        <v>1nnu</v>
       </c>
     </row>
     <row r="30" spans="1:44">
@@ -5278,8 +5315,9 @@
       <c r="AQ30" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="AR30">
-        <v>9</v>
+      <c r="AR30" t="str">
+        <f t="shared" si="0"/>
+        <v>1nnu</v>
       </c>
     </row>
     <row r="31" spans="1:44">
@@ -5412,8 +5450,9 @@
       <c r="AQ31" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="AR31">
-        <v>7</v>
+      <c r="AR31" t="str">
+        <f t="shared" si="0"/>
+        <v>1nnu</v>
       </c>
     </row>
     <row r="32" spans="1:44">
@@ -5546,8 +5585,9 @@
       <c r="AQ32" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="AR32">
-        <v>1</v>
+      <c r="AR32" t="str">
+        <f t="shared" si="0"/>
+        <v>1nnu</v>
       </c>
     </row>
     <row r="33" spans="1:44">
@@ -5680,8 +5720,9 @@
       <c r="AQ33" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="AR33">
-        <v>6</v>
+      <c r="AR33" t="str">
+        <f t="shared" si="0"/>
+        <v>1nnu</v>
       </c>
     </row>
     <row r="34" spans="1:44">
@@ -5814,8 +5855,9 @@
       <c r="AQ34" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="AR34">
-        <v>8</v>
+      <c r="AR34" t="str">
+        <f t="shared" si="0"/>
+        <v>1nnu</v>
       </c>
     </row>
     <row r="35" spans="1:44">
@@ -5948,8 +5990,9 @@
       <c r="AQ35" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="AR35">
-        <v>2</v>
+      <c r="AR35" t="str">
+        <f t="shared" si="0"/>
+        <v>1nnu</v>
       </c>
     </row>
     <row r="36" spans="1:44">
@@ -6082,8 +6125,9 @@
       <c r="AQ36" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="AR36">
-        <v>7</v>
+      <c r="AR36" t="str">
+        <f t="shared" si="0"/>
+        <v>1nnu</v>
       </c>
     </row>
     <row r="37" spans="1:44">
@@ -6216,8 +6260,9 @@
       <c r="AQ37" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="AR37">
-        <v>2</v>
+      <c r="AR37" t="str">
+        <f t="shared" si="0"/>
+        <v>1o2d</v>
       </c>
     </row>
     <row r="38" spans="1:44">
@@ -6350,8 +6395,9 @@
       <c r="AQ38" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="AR38">
-        <v>7</v>
+      <c r="AR38" t="str">
+        <f t="shared" si="0"/>
+        <v>1o2d</v>
       </c>
     </row>
     <row r="39" spans="1:44">
@@ -6484,8 +6530,9 @@
       <c r="AQ39" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="AR39">
-        <v>4</v>
+      <c r="AR39" t="str">
+        <f t="shared" si="0"/>
+        <v>1o2d</v>
       </c>
     </row>
     <row r="40" spans="1:44">
@@ -6618,8 +6665,9 @@
       <c r="AQ40" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="AR40">
-        <v>9</v>
+      <c r="AR40" t="str">
+        <f t="shared" si="0"/>
+        <v>1o2d</v>
       </c>
     </row>
     <row r="41" spans="1:44">
@@ -6752,8 +6800,9 @@
       <c r="AQ41" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="AR41">
-        <v>5</v>
+      <c r="AR41" t="str">
+        <f t="shared" si="0"/>
+        <v>1o2d</v>
       </c>
     </row>
     <row r="42" spans="1:44">
@@ -6886,8 +6935,9 @@
       <c r="AQ42" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="AR42">
-        <v>6</v>
+      <c r="AR42" t="str">
+        <f t="shared" si="0"/>
+        <v>1o2d</v>
       </c>
     </row>
     <row r="43" spans="1:44">
@@ -7020,8 +7070,9 @@
       <c r="AQ43" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="AR43">
-        <v>4</v>
+      <c r="AR43" t="str">
+        <f t="shared" si="0"/>
+        <v>1oaa</v>
       </c>
     </row>
     <row r="44" spans="1:44">
@@ -7154,8 +7205,9 @@
       <c r="AQ44" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="AR44">
-        <v>7</v>
+      <c r="AR44" t="str">
+        <f t="shared" si="0"/>
+        <v>1oaa</v>
       </c>
     </row>
     <row r="45" spans="1:44">
@@ -7288,8 +7340,9 @@
       <c r="AQ45" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="AR45">
-        <v>9</v>
+      <c r="AR45" t="str">
+        <f t="shared" si="0"/>
+        <v>1oaa</v>
       </c>
     </row>
     <row r="46" spans="1:44">
@@ -7422,8 +7475,9 @@
       <c r="AQ46" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="AR46">
-        <v>6</v>
+      <c r="AR46" t="str">
+        <f t="shared" si="0"/>
+        <v>1oaa</v>
       </c>
     </row>
     <row r="47" spans="1:44">
@@ -7556,8 +7610,9 @@
       <c r="AQ47" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="AR47">
-        <v>1</v>
+      <c r="AR47" t="str">
+        <f t="shared" si="0"/>
+        <v>1oaa</v>
       </c>
     </row>
     <row r="48" spans="1:44">
@@ -7690,8 +7745,9 @@
       <c r="AQ48" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="AR48">
-        <v>3</v>
+      <c r="AR48" t="str">
+        <f t="shared" si="0"/>
+        <v>1oaa</v>
       </c>
     </row>
     <row r="49" spans="1:44">
@@ -7824,8 +7880,9 @@
       <c r="AQ49" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="AR49">
-        <v>5</v>
+      <c r="AR49" t="str">
+        <f t="shared" si="0"/>
+        <v>1oaa</v>
       </c>
     </row>
     <row r="50" spans="1:44">
@@ -7958,8 +8015,9 @@
       <c r="AQ50" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="AR50">
-        <v>8</v>
+      <c r="AR50" t="str">
+        <f t="shared" si="0"/>
+        <v>1oaa</v>
       </c>
     </row>
     <row r="51" spans="1:44">
@@ -8092,8 +8150,9 @@
       <c r="AQ51" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="AR51">
-        <v>2</v>
+      <c r="AR51" t="str">
+        <f t="shared" si="0"/>
+        <v>1oaa</v>
       </c>
     </row>
     <row r="52" spans="1:44">
@@ -8226,8 +8285,9 @@
       <c r="AQ52" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="AR52">
-        <v>5</v>
+      <c r="AR52" t="str">
+        <f t="shared" si="0"/>
+        <v>1oaa</v>
       </c>
     </row>
     <row r="53" spans="1:44">
@@ -8360,8 +8420,9 @@
       <c r="AQ53" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="AR53">
-        <v>4</v>
+      <c r="AR53" t="str">
+        <f t="shared" si="0"/>
+        <v>1oaa</v>
       </c>
     </row>
     <row r="54" spans="1:44">
@@ -8494,8 +8555,9 @@
       <c r="AQ54" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="AR54">
-        <v>1</v>
+      <c r="AR54" t="str">
+        <f t="shared" si="0"/>
+        <v>1oaa</v>
       </c>
     </row>
     <row r="55" spans="1:44">
@@ -8628,8 +8690,9 @@
       <c r="AQ55" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="AR55">
-        <v>3</v>
+      <c r="AR55" t="str">
+        <f t="shared" si="0"/>
+        <v>1oaa</v>
       </c>
     </row>
     <row r="56" spans="1:44">
@@ -8762,8 +8825,9 @@
       <c r="AQ56" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="AR56">
-        <v>5</v>
+      <c r="AR56" t="str">
+        <f t="shared" si="0"/>
+        <v>2ag8</v>
       </c>
     </row>
     <row r="57" spans="1:44">
@@ -8896,8 +8960,9 @@
       <c r="AQ57" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="AR57">
-        <v>3</v>
+      <c r="AR57" t="str">
+        <f t="shared" si="0"/>
+        <v>2ag8</v>
       </c>
     </row>
     <row r="58" spans="1:44">
@@ -9030,8 +9095,9 @@
       <c r="AQ58" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="AR58">
-        <v>6</v>
+      <c r="AR58" t="str">
+        <f t="shared" si="0"/>
+        <v>2ag8</v>
       </c>
     </row>
     <row r="59" spans="1:44">
@@ -9164,8 +9230,9 @@
       <c r="AQ59" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="AR59">
-        <v>8</v>
+      <c r="AR59" t="str">
+        <f t="shared" si="0"/>
+        <v>2ag8</v>
       </c>
     </row>
     <row r="60" spans="1:44">
@@ -9298,8 +9365,9 @@
       <c r="AQ60" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="AR60">
-        <v>7</v>
+      <c r="AR60" t="str">
+        <f t="shared" si="0"/>
+        <v>2ag8</v>
       </c>
     </row>
     <row r="61" spans="1:44">
@@ -9432,8 +9500,9 @@
       <c r="AQ61" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="AR61">
-        <v>4</v>
+      <c r="AR61" t="str">
+        <f t="shared" si="0"/>
+        <v>2ag8</v>
       </c>
     </row>
     <row r="62" spans="1:44">
@@ -9566,8 +9635,9 @@
       <c r="AQ62" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="AR62">
-        <v>1</v>
+      <c r="AR62" t="str">
+        <f t="shared" si="0"/>
+        <v>2ag8</v>
       </c>
     </row>
     <row r="63" spans="1:44">
@@ -9700,8 +9770,9 @@
       <c r="AQ63" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="AR63">
-        <v>9</v>
+      <c r="AR63" t="str">
+        <f t="shared" si="0"/>
+        <v>2ag8</v>
       </c>
     </row>
     <row r="64" spans="1:44">
@@ -9834,8 +9905,9 @@
       <c r="AQ64" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="AR64">
-        <v>2</v>
+      <c r="AR64" t="str">
+        <f t="shared" si="0"/>
+        <v>2ag8</v>
       </c>
     </row>
     <row r="65" spans="1:44">
@@ -9968,8 +10040,9 @@
       <c r="AQ65" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="AR65">
-        <v>1</v>
+      <c r="AR65" t="str">
+        <f t="shared" si="0"/>
+        <v>2d2i</v>
       </c>
     </row>
     <row r="66" spans="1:44">
@@ -10102,8 +10175,9 @@
       <c r="AQ66" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="AR66">
-        <v>4</v>
+      <c r="AR66" t="str">
+        <f t="shared" si="0"/>
+        <v>2d2i</v>
       </c>
     </row>
     <row r="67" spans="1:44">
@@ -10236,8 +10310,9 @@
       <c r="AQ67" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="AR67">
-        <v>7</v>
+      <c r="AR67" t="str">
+        <f t="shared" ref="AR67:AR130" si="1">MID(AP67,1,4)</f>
+        <v>2d2i</v>
       </c>
     </row>
     <row r="68" spans="1:44">
@@ -10370,8 +10445,9 @@
       <c r="AQ68" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="AR68">
-        <v>2</v>
+      <c r="AR68" t="str">
+        <f t="shared" si="1"/>
+        <v>2d2i</v>
       </c>
     </row>
     <row r="69" spans="1:44">
@@ -10504,8 +10580,9 @@
       <c r="AQ69" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="AR69">
-        <v>6</v>
+      <c r="AR69" t="str">
+        <f t="shared" si="1"/>
+        <v>2d2i</v>
       </c>
     </row>
     <row r="70" spans="1:44">
@@ -10638,8 +10715,9 @@
       <c r="AQ70" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="AR70">
-        <v>1</v>
+      <c r="AR70" t="str">
+        <f t="shared" si="1"/>
+        <v>2d2i</v>
       </c>
     </row>
     <row r="71" spans="1:44">
@@ -10772,8 +10850,9 @@
       <c r="AQ71" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="AR71">
-        <v>1</v>
+      <c r="AR71" t="str">
+        <f t="shared" si="1"/>
+        <v>2f1k</v>
       </c>
     </row>
     <row r="72" spans="1:44">
@@ -10906,8 +10985,9 @@
       <c r="AQ72" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="AR72">
-        <v>5</v>
+      <c r="AR72" t="str">
+        <f t="shared" si="1"/>
+        <v>2f1k</v>
       </c>
     </row>
     <row r="73" spans="1:44">
@@ -11040,8 +11120,9 @@
       <c r="AQ73" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="AR73">
-        <v>6</v>
+      <c r="AR73" t="str">
+        <f t="shared" si="1"/>
+        <v>2f1k</v>
       </c>
     </row>
     <row r="74" spans="1:44">
@@ -11174,8 +11255,9 @@
       <c r="AQ74" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="AR74">
-        <v>4</v>
+      <c r="AR74" t="str">
+        <f t="shared" si="1"/>
+        <v>2v6g</v>
       </c>
     </row>
     <row r="75" spans="1:44">
@@ -11308,8 +11390,9 @@
       <c r="AQ75" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="AR75">
-        <v>2</v>
+      <c r="AR75" t="str">
+        <f t="shared" si="1"/>
+        <v>2v6g</v>
       </c>
     </row>
     <row r="76" spans="1:44">
@@ -11442,8 +11525,9 @@
       <c r="AQ76" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="AR76">
-        <v>3</v>
+      <c r="AR76" t="str">
+        <f t="shared" si="1"/>
+        <v>2v6g</v>
       </c>
     </row>
     <row r="77" spans="1:44">
@@ -11576,8 +11660,9 @@
       <c r="AQ77" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="AR77">
-        <v>5</v>
+      <c r="AR77" t="str">
+        <f t="shared" si="1"/>
+        <v>2v6g</v>
       </c>
     </row>
     <row r="78" spans="1:44">
@@ -11710,8 +11795,9 @@
       <c r="AQ78" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="AR78">
-        <v>6</v>
+      <c r="AR78" t="str">
+        <f t="shared" si="1"/>
+        <v>2v6g</v>
       </c>
     </row>
     <row r="79" spans="1:44">
@@ -11844,8 +11930,9 @@
       <c r="AQ79" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="AR79">
-        <v>7</v>
+      <c r="AR79" t="str">
+        <f t="shared" si="1"/>
+        <v>2v6g</v>
       </c>
     </row>
     <row r="80" spans="1:44">
@@ -11978,8 +12065,9 @@
       <c r="AQ80" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="AR80">
-        <v>9</v>
+      <c r="AR80" t="str">
+        <f t="shared" si="1"/>
+        <v>2v6g</v>
       </c>
     </row>
     <row r="81" spans="1:44">
@@ -12112,8 +12200,9 @@
       <c r="AQ81" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="AR81">
-        <v>8</v>
+      <c r="AR81" t="str">
+        <f t="shared" si="1"/>
+        <v>2v6g</v>
       </c>
     </row>
     <row r="82" spans="1:44">
@@ -12246,8 +12335,9 @@
       <c r="AQ82" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="AR82">
-        <v>1</v>
+      <c r="AR82" t="str">
+        <f t="shared" si="1"/>
+        <v>2v6g</v>
       </c>
     </row>
     <row r="83" spans="1:44">
@@ -12380,8 +12470,9 @@
       <c r="AQ83" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="AR83">
-        <v>4</v>
+      <c r="AR83" t="str">
+        <f t="shared" si="1"/>
+        <v>2v6g</v>
       </c>
     </row>
     <row r="84" spans="1:44">
@@ -12514,8 +12605,9 @@
       <c r="AQ84" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="AR84">
-        <v>6</v>
+      <c r="AR84" t="str">
+        <f t="shared" si="1"/>
+        <v>3jyo</v>
       </c>
     </row>
     <row r="85" spans="1:44">
@@ -12648,8 +12740,9 @@
       <c r="AQ85" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="AR85">
-        <v>2</v>
+      <c r="AR85" t="str">
+        <f t="shared" si="1"/>
+        <v>3jyo</v>
       </c>
     </row>
     <row r="86" spans="1:44">
@@ -12782,8 +12875,9 @@
       <c r="AQ86" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="AR86">
-        <v>1</v>
+      <c r="AR86" t="str">
+        <f t="shared" si="1"/>
+        <v>3jyo</v>
       </c>
     </row>
     <row r="87" spans="1:44">
@@ -12916,8 +13010,9 @@
       <c r="AQ87" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="AR87">
-        <v>4</v>
+      <c r="AR87" t="str">
+        <f t="shared" si="1"/>
+        <v>3jyo</v>
       </c>
     </row>
     <row r="88" spans="1:44">
@@ -13050,8 +13145,9 @@
       <c r="AQ88" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="AR88">
-        <v>7</v>
+      <c r="AR88" t="str">
+        <f t="shared" si="1"/>
+        <v>3jyo</v>
       </c>
     </row>
     <row r="89" spans="1:44">
@@ -13184,8 +13280,9 @@
       <c r="AQ89" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="AR89">
-        <v>5</v>
+      <c r="AR89" t="str">
+        <f t="shared" si="1"/>
+        <v>3jyo</v>
       </c>
     </row>
     <row r="90" spans="1:44">
@@ -13318,8 +13415,9 @@
       <c r="AQ90" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="AR90">
-        <v>1</v>
+      <c r="AR90" t="str">
+        <f t="shared" si="1"/>
+        <v>3jyo</v>
       </c>
     </row>
     <row r="91" spans="1:44">
@@ -13452,8 +13550,9 @@
       <c r="AQ91" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="AR91">
-        <v>6</v>
+      <c r="AR91" t="str">
+        <f t="shared" si="1"/>
+        <v>3jyo</v>
       </c>
     </row>
     <row r="92" spans="1:44">
@@ -13586,8 +13685,9 @@
       <c r="AQ92" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="AR92">
-        <v>7</v>
+      <c r="AR92" t="str">
+        <f t="shared" si="1"/>
+        <v>3jyo</v>
       </c>
     </row>
     <row r="93" spans="1:44">
@@ -13720,8 +13820,9 @@
       <c r="AQ93" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="AR93">
-        <v>8</v>
+      <c r="AR93" t="str">
+        <f t="shared" si="1"/>
+        <v>3jyo</v>
       </c>
     </row>
     <row r="94" spans="1:44">
@@ -13854,8 +13955,9 @@
       <c r="AQ94" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="AR94">
-        <v>9</v>
+      <c r="AR94" t="str">
+        <f t="shared" si="1"/>
+        <v>3jyo</v>
       </c>
     </row>
     <row r="95" spans="1:44">
@@ -13988,8 +14090,9 @@
       <c r="AQ95" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="AR95">
-        <v>4</v>
+      <c r="AR95" t="str">
+        <f t="shared" si="1"/>
+        <v>3jyo</v>
       </c>
     </row>
     <row r="96" spans="1:44">
@@ -14122,8 +14225,9 @@
       <c r="AQ96" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="AR96">
-        <v>5</v>
+      <c r="AR96" t="str">
+        <f t="shared" si="1"/>
+        <v>3jyo</v>
       </c>
     </row>
     <row r="97" spans="1:44">
@@ -14256,8 +14360,9 @@
       <c r="AQ97" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="AR97">
-        <v>3</v>
+      <c r="AR97" t="str">
+        <f t="shared" si="1"/>
+        <v>3jyo</v>
       </c>
     </row>
     <row r="98" spans="1:44">
@@ -14390,8 +14495,9 @@
       <c r="AQ98" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="AR98">
-        <v>2</v>
+      <c r="AR98" t="str">
+        <f t="shared" si="1"/>
+        <v>3jyo</v>
       </c>
     </row>
     <row r="99" spans="1:44">
@@ -14524,8 +14630,9 @@
       <c r="AQ99" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="AR99">
-        <v>4</v>
+      <c r="AR99" t="str">
+        <f t="shared" si="1"/>
+        <v>3jyo</v>
       </c>
     </row>
     <row r="100" spans="1:44">
@@ -14658,8 +14765,9 @@
       <c r="AQ100" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="AR100">
-        <v>3</v>
+      <c r="AR100" t="str">
+        <f t="shared" si="1"/>
+        <v>3jyo</v>
       </c>
     </row>
     <row r="101" spans="1:44">
@@ -14792,8 +14900,9 @@
       <c r="AQ101" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="AR101">
-        <v>9</v>
+      <c r="AR101" t="str">
+        <f t="shared" si="1"/>
+        <v>3jyo</v>
       </c>
     </row>
     <row r="102" spans="1:44">
@@ -14926,8 +15035,9 @@
       <c r="AQ102" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="AR102">
-        <v>2</v>
+      <c r="AR102" t="str">
+        <f t="shared" si="1"/>
+        <v>3jyo</v>
       </c>
     </row>
     <row r="103" spans="1:44">
@@ -15060,8 +15170,9 @@
       <c r="AQ103" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="AR103">
-        <v>1</v>
+      <c r="AR103" t="str">
+        <f t="shared" si="1"/>
+        <v>3jyo</v>
       </c>
     </row>
     <row r="104" spans="1:44">
@@ -15194,8 +15305,9 @@
       <c r="AQ104" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="AR104">
-        <v>8</v>
+      <c r="AR104" t="str">
+        <f t="shared" si="1"/>
+        <v>3jyo</v>
       </c>
     </row>
     <row r="105" spans="1:44">
@@ -15328,8 +15440,9 @@
       <c r="AQ105" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="AR105">
-        <v>6</v>
+      <c r="AR105" t="str">
+        <f t="shared" si="1"/>
+        <v>3jyo</v>
       </c>
     </row>
     <row r="106" spans="1:44">
@@ -15462,8 +15575,9 @@
       <c r="AQ106" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="AR106">
-        <v>4</v>
+      <c r="AR106" t="str">
+        <f t="shared" si="1"/>
+        <v>3orf</v>
       </c>
     </row>
     <row r="107" spans="1:44">
@@ -15596,8 +15710,9 @@
       <c r="AQ107" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="AR107">
-        <v>3</v>
+      <c r="AR107" t="str">
+        <f t="shared" si="1"/>
+        <v>3orf</v>
       </c>
     </row>
     <row r="108" spans="1:44">
@@ -15730,8 +15845,9 @@
       <c r="AQ108" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="AR108">
-        <v>9</v>
+      <c r="AR108" t="str">
+        <f t="shared" si="1"/>
+        <v>3orf</v>
       </c>
     </row>
     <row r="109" spans="1:44">
@@ -15864,8 +15980,9 @@
       <c r="AQ109" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="AR109">
-        <v>1</v>
+      <c r="AR109" t="str">
+        <f t="shared" si="1"/>
+        <v>3orf</v>
       </c>
     </row>
     <row r="110" spans="1:44">
@@ -15998,8 +16115,9 @@
       <c r="AQ110" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="AR110">
-        <v>4</v>
+      <c r="AR110" t="str">
+        <f t="shared" si="1"/>
+        <v>3orf</v>
       </c>
     </row>
     <row r="111" spans="1:44">
@@ -16132,8 +16250,9 @@
       <c r="AQ111" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="AR111">
-        <v>9</v>
+      <c r="AR111" t="str">
+        <f t="shared" si="1"/>
+        <v>4bms</v>
       </c>
     </row>
     <row r="112" spans="1:44">
@@ -16266,8 +16385,9 @@
       <c r="AQ112" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="AR112">
-        <v>5</v>
+      <c r="AR112" t="str">
+        <f t="shared" si="1"/>
+        <v>4bms</v>
       </c>
     </row>
     <row r="113" spans="1:44">
@@ -16400,8 +16520,9 @@
       <c r="AQ113" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="AR113">
-        <v>1</v>
+      <c r="AR113" t="str">
+        <f t="shared" si="1"/>
+        <v>4bms</v>
       </c>
     </row>
     <row r="114" spans="1:44">
@@ -16534,8 +16655,9 @@
       <c r="AQ114" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="AR114">
-        <v>3</v>
+      <c r="AR114" t="str">
+        <f t="shared" si="1"/>
+        <v>4bms</v>
       </c>
     </row>
     <row r="115" spans="1:44">
@@ -16668,8 +16790,9 @@
       <c r="AQ115" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="AR115">
-        <v>8</v>
+      <c r="AR115" t="str">
+        <f t="shared" si="1"/>
+        <v>4bms</v>
       </c>
     </row>
     <row r="116" spans="1:44">
@@ -16802,8 +16925,9 @@
       <c r="AQ116" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="AR116">
-        <v>6</v>
+      <c r="AR116" t="str">
+        <f t="shared" si="1"/>
+        <v>4bms</v>
       </c>
     </row>
     <row r="117" spans="1:44">
@@ -16936,8 +17060,9 @@
       <c r="AQ117" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="AR117">
-        <v>2</v>
+      <c r="AR117" t="str">
+        <f t="shared" si="1"/>
+        <v>4bms</v>
       </c>
     </row>
     <row r="118" spans="1:44">
@@ -17070,8 +17195,9 @@
       <c r="AQ118" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="AR118">
-        <v>1</v>
+      <c r="AR118" t="str">
+        <f t="shared" si="1"/>
+        <v>4bms</v>
       </c>
     </row>
     <row r="119" spans="1:44">
@@ -17204,8 +17330,9 @@
       <c r="AQ119" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="AR119">
-        <v>4</v>
+      <c r="AR119" t="str">
+        <f t="shared" si="1"/>
+        <v>4bms</v>
       </c>
     </row>
     <row r="120" spans="1:44">
@@ -17338,8 +17465,9 @@
       <c r="AQ120" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="AR120">
-        <v>9</v>
+      <c r="AR120" t="str">
+        <f t="shared" si="1"/>
+        <v>4bms</v>
       </c>
     </row>
     <row r="121" spans="1:44">
@@ -17472,8 +17600,9 @@
       <c r="AQ121" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="AR121">
-        <v>2</v>
+      <c r="AR121" t="str">
+        <f t="shared" si="1"/>
+        <v>4bms</v>
       </c>
     </row>
     <row r="122" spans="1:44">
@@ -17606,8 +17735,9 @@
       <c r="AQ122" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="AR122">
-        <v>7</v>
+      <c r="AR122" t="str">
+        <f t="shared" si="1"/>
+        <v>4bms</v>
       </c>
     </row>
     <row r="123" spans="1:44">
@@ -17740,8 +17870,9 @@
       <c r="AQ123" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="AR123">
-        <v>7</v>
+      <c r="AR123" t="str">
+        <f t="shared" si="1"/>
+        <v>4bms</v>
       </c>
     </row>
     <row r="124" spans="1:44">
@@ -17874,8 +18005,9 @@
       <c r="AQ124" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="AR124">
-        <v>3</v>
+      <c r="AR124" t="str">
+        <f t="shared" si="1"/>
+        <v>4bms</v>
       </c>
     </row>
     <row r="125" spans="1:44">
@@ -18008,8 +18140,9 @@
       <c r="AQ125" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="AR125">
-        <v>1</v>
+      <c r="AR125" t="str">
+        <f t="shared" si="1"/>
+        <v>4bms</v>
       </c>
     </row>
     <row r="126" spans="1:44">
@@ -18142,8 +18275,9 @@
       <c r="AQ126" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="AR126">
-        <v>4</v>
+      <c r="AR126" t="str">
+        <f t="shared" si="1"/>
+        <v>4bms</v>
       </c>
     </row>
     <row r="127" spans="1:44">
@@ -18276,8 +18410,9 @@
       <c r="AQ127" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="AR127">
-        <v>8</v>
+      <c r="AR127" t="str">
+        <f t="shared" si="1"/>
+        <v>4bms</v>
       </c>
     </row>
     <row r="128" spans="1:44">
@@ -18410,8 +18545,9 @@
       <c r="AQ128" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="AR128">
-        <v>9</v>
+      <c r="AR128" t="str">
+        <f t="shared" si="1"/>
+        <v>4bms</v>
       </c>
     </row>
     <row r="129" spans="1:44">
@@ -18544,8 +18680,9 @@
       <c r="AQ129" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="AR129">
-        <v>6</v>
+      <c r="AR129" t="str">
+        <f t="shared" si="1"/>
+        <v>4bms</v>
       </c>
     </row>
     <row r="130" spans="1:44">
@@ -18678,8 +18815,9 @@
       <c r="AQ130" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="AR130">
-        <v>5</v>
+      <c r="AR130" t="str">
+        <f t="shared" si="1"/>
+        <v>4bms</v>
       </c>
     </row>
     <row r="131" spans="1:44">
@@ -18812,8 +18950,9 @@
       <c r="AQ131" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="AR131">
-        <v>2</v>
+      <c r="AR131" t="str">
+        <f t="shared" ref="AR131:AR164" si="2">MID(AP131,1,4)</f>
+        <v>4bms</v>
       </c>
     </row>
     <row r="132" spans="1:44">
@@ -18946,8 +19085,9 @@
       <c r="AQ132" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="AR132">
-        <v>6</v>
+      <c r="AR132" t="str">
+        <f t="shared" si="2"/>
+        <v>4bms</v>
       </c>
     </row>
     <row r="133" spans="1:44">
@@ -19080,8 +19220,9 @@
       <c r="AQ133" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="AR133">
-        <v>3</v>
+      <c r="AR133" t="str">
+        <f t="shared" si="2"/>
+        <v>4bms</v>
       </c>
     </row>
     <row r="134" spans="1:44">
@@ -19214,8 +19355,9 @@
       <c r="AQ134" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="AR134">
-        <v>6</v>
+      <c r="AR134" t="str">
+        <f t="shared" si="2"/>
+        <v>4bms</v>
       </c>
     </row>
     <row r="135" spans="1:44">
@@ -19348,8 +19490,9 @@
       <c r="AQ135" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="AR135">
-        <v>1</v>
+      <c r="AR135" t="str">
+        <f t="shared" si="2"/>
+        <v>4bms</v>
       </c>
     </row>
     <row r="136" spans="1:44">
@@ -19482,8 +19625,9 @@
       <c r="AQ136" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="AR136">
-        <v>2</v>
+      <c r="AR136" t="str">
+        <f t="shared" si="2"/>
+        <v>4bms</v>
       </c>
     </row>
     <row r="137" spans="1:44">
@@ -19616,8 +19760,9 @@
       <c r="AQ137" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="AR137">
-        <v>3</v>
+      <c r="AR137" t="str">
+        <f t="shared" si="2"/>
+        <v>4bms</v>
       </c>
     </row>
     <row r="138" spans="1:44">
@@ -19750,8 +19895,9 @@
       <c r="AQ138" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="AR138">
-        <v>5</v>
+      <c r="AR138" t="str">
+        <f t="shared" si="2"/>
+        <v>4bms</v>
       </c>
     </row>
     <row r="139" spans="1:44">
@@ -19884,8 +20030,9 @@
       <c r="AQ139" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="AR139">
-        <v>8</v>
+      <c r="AR139" t="str">
+        <f t="shared" si="2"/>
+        <v>4bms</v>
       </c>
     </row>
     <row r="140" spans="1:44">
@@ -20018,8 +20165,9 @@
       <c r="AQ140" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="AR140">
-        <v>8</v>
+      <c r="AR140" t="str">
+        <f t="shared" si="2"/>
+        <v>4bmv</v>
       </c>
     </row>
     <row r="141" spans="1:44">
@@ -20152,8 +20300,9 @@
       <c r="AQ141" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="AR141">
-        <v>7</v>
+      <c r="AR141" t="str">
+        <f t="shared" si="2"/>
+        <v>4bmv</v>
       </c>
     </row>
     <row r="142" spans="1:44">
@@ -20286,8 +20435,9 @@
       <c r="AQ142" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="AR142">
-        <v>1</v>
+      <c r="AR142" t="str">
+        <f t="shared" si="2"/>
+        <v>4bmv</v>
       </c>
     </row>
     <row r="143" spans="1:44">
@@ -20420,8 +20570,9 @@
       <c r="AQ143" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="AR143">
-        <v>2</v>
+      <c r="AR143" t="str">
+        <f t="shared" si="2"/>
+        <v>4bmv</v>
       </c>
     </row>
     <row r="144" spans="1:44">
@@ -20554,8 +20705,9 @@
       <c r="AQ144" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="AR144">
-        <v>6</v>
+      <c r="AR144" t="str">
+        <f t="shared" si="2"/>
+        <v>4bmv</v>
       </c>
     </row>
     <row r="145" spans="1:44">
@@ -20688,8 +20840,9 @@
       <c r="AQ145" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="AR145">
-        <v>3</v>
+      <c r="AR145" t="str">
+        <f t="shared" si="2"/>
+        <v>4bmv</v>
       </c>
     </row>
     <row r="146" spans="1:44">
@@ -20822,8 +20975,9 @@
       <c r="AQ146" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="AR146">
-        <v>4</v>
+      <c r="AR146" t="str">
+        <f t="shared" si="2"/>
+        <v>4bmv</v>
       </c>
     </row>
     <row r="147" spans="1:44">
@@ -20956,8 +21110,9 @@
       <c r="AQ147" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="AR147">
-        <v>9</v>
+      <c r="AR147" t="str">
+        <f t="shared" si="2"/>
+        <v>4bmv</v>
       </c>
     </row>
     <row r="148" spans="1:44">
@@ -21090,8 +21245,9 @@
       <c r="AQ148" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="AR148">
-        <v>5</v>
+      <c r="AR148" t="str">
+        <f t="shared" si="2"/>
+        <v>4bmv</v>
       </c>
     </row>
     <row r="149" spans="1:44">
@@ -21224,8 +21380,9 @@
       <c r="AQ149" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="AR149">
-        <v>5</v>
+      <c r="AR149" t="str">
+        <f t="shared" si="2"/>
+        <v>4bmv</v>
       </c>
     </row>
     <row r="150" spans="1:44">
@@ -21358,8 +21515,9 @@
       <c r="AQ150" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="AR150">
-        <v>7</v>
+      <c r="AR150" t="str">
+        <f t="shared" si="2"/>
+        <v>4bmv</v>
       </c>
     </row>
     <row r="151" spans="1:44">
@@ -21492,8 +21650,9 @@
       <c r="AQ151" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="AR151">
-        <v>8</v>
+      <c r="AR151" t="str">
+        <f t="shared" si="2"/>
+        <v>4bmv</v>
       </c>
     </row>
     <row r="152" spans="1:44">
@@ -21626,8 +21785,9 @@
       <c r="AQ152" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="AR152">
-        <v>1</v>
+      <c r="AR152" t="str">
+        <f t="shared" si="2"/>
+        <v>4bmv</v>
       </c>
     </row>
     <row r="153" spans="1:44">
@@ -21760,8 +21920,9 @@
       <c r="AQ153" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="AR153">
-        <v>9</v>
+      <c r="AR153" t="str">
+        <f t="shared" si="2"/>
+        <v>4bmv</v>
       </c>
     </row>
     <row r="154" spans="1:44">
@@ -21894,8 +22055,9 @@
       <c r="AQ154" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="AR154">
-        <v>4</v>
+      <c r="AR154" t="str">
+        <f t="shared" si="2"/>
+        <v>4bmv</v>
       </c>
     </row>
     <row r="155" spans="1:44">
@@ -22028,8 +22190,9 @@
       <c r="AQ155" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="AR155">
-        <v>3</v>
+      <c r="AR155" t="str">
+        <f t="shared" si="2"/>
+        <v>4bmv</v>
       </c>
     </row>
     <row r="156" spans="1:44">
@@ -22162,8 +22325,9 @@
       <c r="AQ156" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="AR156">
-        <v>6</v>
+      <c r="AR156" t="str">
+        <f t="shared" si="2"/>
+        <v>4bmv</v>
       </c>
     </row>
     <row r="157" spans="1:44">
@@ -22296,8 +22460,9 @@
       <c r="AQ157" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="AR157">
-        <v>4</v>
+      <c r="AR157" t="str">
+        <f t="shared" si="2"/>
+        <v>4bmv</v>
       </c>
     </row>
     <row r="158" spans="1:44">
@@ -22430,8 +22595,9 @@
       <c r="AQ158" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="AR158">
-        <v>9</v>
+      <c r="AR158" t="str">
+        <f t="shared" si="2"/>
+        <v>4bmv</v>
       </c>
     </row>
     <row r="159" spans="1:44">
@@ -22564,8 +22730,9 @@
       <c r="AQ159" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="AR159">
-        <v>8</v>
+      <c r="AR159" t="str">
+        <f t="shared" si="2"/>
+        <v>4bmv</v>
       </c>
     </row>
     <row r="160" spans="1:44">
@@ -22698,8 +22865,9 @@
       <c r="AQ160" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="AR160">
-        <v>7</v>
+      <c r="AR160" t="str">
+        <f t="shared" si="2"/>
+        <v>4bmv</v>
       </c>
     </row>
     <row r="161" spans="1:44">
@@ -22832,8 +23000,9 @@
       <c r="AQ161" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="AR161">
-        <v>3</v>
+      <c r="AR161" t="str">
+        <f t="shared" si="2"/>
+        <v>4bmv</v>
       </c>
     </row>
     <row r="162" spans="1:44">
@@ -22966,8 +23135,9 @@
       <c r="AQ162" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="AR162">
-        <v>2</v>
+      <c r="AR162" t="str">
+        <f t="shared" si="2"/>
+        <v>4bmv</v>
       </c>
     </row>
     <row r="163" spans="1:44">
@@ -23100,8 +23270,9 @@
       <c r="AQ163" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="AR163">
-        <v>1</v>
+      <c r="AR163" t="str">
+        <f t="shared" si="2"/>
+        <v>4bmv</v>
       </c>
     </row>
     <row r="164" spans="1:44">
@@ -23234,8 +23405,9 @@
       <c r="AQ164" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="AR164">
-        <v>5</v>
+      <c r="AR164" t="str">
+        <f t="shared" si="2"/>
+        <v>4bmv</v>
       </c>
     </row>
   </sheetData>

</xml_diff>